<commit_message>
Add updated files for report.docx
</commit_message>
<xml_diff>
--- a/Reports/GanttChart stylized.xlsx
+++ b/Reports/GanttChart stylized.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joao\Documents\GitHub\CS_5150\Reports\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -77,9 +77,6 @@
     <t>Presentation #1</t>
   </si>
   <si>
-    <t>Usability Test</t>
-  </si>
-  <si>
     <t>Implementation study of structure of files - phase 2</t>
   </si>
   <si>
@@ -92,22 +89,25 @@
     <t>Presentation #2</t>
   </si>
   <si>
-    <t>User testing</t>
-  </si>
-  <si>
-    <t>Client testing</t>
-  </si>
-  <si>
     <t>Final presentation #3</t>
   </si>
   <si>
-    <t>Test the enhanced product - phase 2</t>
-  </si>
-  <si>
     <t>In progress</t>
   </si>
   <si>
     <t>User Interface Design - phase 1</t>
+  </si>
+  <si>
+    <t>User testing 1</t>
+  </si>
+  <si>
+    <t>Client testing 1</t>
+  </si>
+  <si>
+    <t>User testing 2</t>
+  </si>
+  <si>
+    <t>Client testing 2</t>
   </si>
 </sst>
 </file>
@@ -391,7 +391,7 @@
                   <c:v>Presentation #1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>Usability Test</c:v>
+                  <c:v>User testing 1</c:v>
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>Implementation study of structure of files - phase 2</c:v>
@@ -400,7 +400,7 @@
                   <c:v>Iterative implementation - phase 2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>Test the enhanced product - phase 2</c:v>
+                  <c:v>Client testing 1</c:v>
                 </c:pt>
                 <c:pt idx="9">
                   <c:v>Presentation #2</c:v>
@@ -412,10 +412,10 @@
                   <c:v>Configuration text editor</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>User testing</c:v>
+                  <c:v>User testing 2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>Client testing</c:v>
+                  <c:v>Client testing 2</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>Review of final project</c:v>
@@ -860,8 +860,8 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="1577864368"/>
-        <c:axId val="1577864912"/>
+        <c:axId val="1078714016"/>
+        <c:axId val="1259199184"/>
         <c:extLst>
           <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
             <c15:filteredBarSeries>
@@ -924,7 +924,7 @@
                         <c:v>Presentation #1</c:v>
                       </c:pt>
                       <c:pt idx="5">
-                        <c:v>Usability Test</c:v>
+                        <c:v>User testing 1</c:v>
                       </c:pt>
                       <c:pt idx="6">
                         <c:v>Implementation study of structure of files - phase 2</c:v>
@@ -933,7 +933,7 @@
                         <c:v>Iterative implementation - phase 2</c:v>
                       </c:pt>
                       <c:pt idx="8">
-                        <c:v>Test the enhanced product - phase 2</c:v>
+                        <c:v>Client testing 1</c:v>
                       </c:pt>
                       <c:pt idx="9">
                         <c:v>Presentation #2</c:v>
@@ -945,10 +945,10 @@
                         <c:v>Configuration text editor</c:v>
                       </c:pt>
                       <c:pt idx="12">
-                        <c:v>User testing</c:v>
+                        <c:v>User testing 2</c:v>
                       </c:pt>
                       <c:pt idx="13">
-                        <c:v>Client testing</c:v>
+                        <c:v>Client testing 2</c:v>
                       </c:pt>
                       <c:pt idx="14">
                         <c:v>Review of final project</c:v>
@@ -1037,7 +1037,7 @@
         </c:extLst>
       </c:barChart>
       <c:catAx>
-        <c:axId val="1577864368"/>
+        <c:axId val="1078714016"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -1088,7 +1088,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1577864912"/>
+        <c:crossAx val="1259199184"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1096,7 +1096,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1577864912"/>
+        <c:axId val="1259199184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="42350"/>
@@ -1157,7 +1157,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1577864368"/>
+        <c:crossAx val="1078714016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
         <c:majorUnit val="7"/>
@@ -2052,8 +2052,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2143,7 +2143,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4" s="12">
         <v>42272</v>
@@ -2166,7 +2166,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="11" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C5" s="12">
         <v>42273</v>
@@ -2212,7 +2212,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="11" t="s">
-        <v>17</v>
+        <v>24</v>
       </c>
       <c r="C7" s="12">
         <v>42303</v>
@@ -2235,7 +2235,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="11" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C8" s="12">
         <v>42296</v>
@@ -2258,7 +2258,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="12">
         <v>42293</v>
@@ -2304,7 +2304,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="11" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C11" s="12">
         <v>42310</v>
@@ -2365,7 +2365,7 @@
         <v>4</v>
       </c>
       <c r="G13" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2373,7 +2373,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="13" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="C14" s="14">
         <v>42315</v>
@@ -2388,7 +2388,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2396,7 +2396,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="14" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="C15" s="14">
         <v>42322</v>
@@ -2411,7 +2411,7 @@
         <v>2</v>
       </c>
       <c r="G15" s="13" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.4">
@@ -2442,7 +2442,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17" s="16">
         <v>42330</v>

</xml_diff>